<commit_message>
some improvements I think... can't remember what all
</commit_message>
<xml_diff>
--- a/cycle_counts.xlsx
+++ b/cycle_counts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Projects\CNC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0AF8652-EAB5-4E69-972F-C73B5D3FCA41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7EED8B-10FA-45E0-B346-E6423FA2FA1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC3E716-96DC-4B36-BCEA-EA55029617FE}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>F</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>mm/sec</t>
   </si>
@@ -65,19 +62,52 @@
     <t>step per usec</t>
   </si>
   <si>
+    <t>step/sec</t>
+  </si>
+  <si>
+    <t>mm/usec</t>
+  </si>
+  <si>
+    <t>cpu/usec</t>
+  </si>
+  <si>
+    <t>usec/cpu</t>
+  </si>
+  <si>
+    <t>Feedrate mm/min</t>
+  </si>
+  <si>
+    <t>usec per step</t>
+  </si>
+  <si>
+    <t>cpu per step</t>
+  </si>
+  <si>
+    <t>rev/sec</t>
+  </si>
+  <si>
+    <t>mm per step</t>
+  </si>
+  <si>
+    <t>count:</t>
+  </si>
+  <si>
+    <t>timer_us:</t>
+  </si>
+  <si>
+    <t>prescale</t>
+  </si>
+  <si>
+    <t>timer val</t>
+  </si>
+  <si>
     <t>usec</t>
   </si>
   <si>
-    <t>cycles per usec</t>
-  </si>
-  <si>
-    <t>step/sec</t>
-  </si>
-  <si>
-    <t>cycles per msec</t>
-  </si>
-  <si>
-    <t>cycles per step</t>
+    <t>sec</t>
+  </si>
+  <si>
+    <t>cpu cycles</t>
   </si>
 </sst>
 </file>
@@ -429,151 +459,432 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4CAD55-91D2-4B4D-A746-B3A215B9AE97}">
-  <dimension ref="B2:F15"/>
+  <dimension ref="B2:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>1200</v>
+        <v>5400</v>
       </c>
       <c r="D2">
-        <f>D3*60</f>
-        <v>1200</v>
+        <v>2100</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>16000000</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>200</v>
+      </c>
+      <c r="L2">
+        <f>PI()*11</f>
+        <v>34.557519189487721</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <f>C2/60</f>
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="D3">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <f>1/F2</f>
         <v>6.2499999999999997E-8</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J8" si="0">$J$2*I3</f>
+        <v>200</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K8" si="1">$L$2/J3</f>
+        <v>0.17278759594743862</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L8" si="2">K3*1000</f>
+        <v>172.7875959474386</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>C3/1000</f>
+        <v>0.09</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <f>F3/(10^-6)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>8.6393797973719308E-2</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>86.393797973719302</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <f>C3/(10^6)</f>
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <f>1/F4</f>
+        <v>16</v>
+      </c>
+      <c r="I5">
         <v>4</v>
       </c>
-      <c r="C4">
-        <f>C3/100</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>4.3196898986859654E-2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>43.196898986859651</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>2.1598449493429827E-2</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>21.598449493429825</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>16</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>1.0799224746714913E-2</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>10.799224746714913</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C8">
+        <v>1600</v>
+      </c>
+      <c r="F8">
+        <f>C13/100</f>
+        <v>180</v>
+      </c>
+      <c r="I8">
+        <v>32</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>6400</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>5.3996123733574567E-3</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>5.3996123733574564</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <f>C8/C7</f>
+        <v>200</v>
+      </c>
+      <c r="F9">
+        <f>C13/(10^6)</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <f>1/C9</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D10">
+        <f>C10*1000</f>
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <f>L2/C7</f>
+        <v>4.3196898986859651</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f>D2*4</f>
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <f>C13/C8</f>
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <f>C3*C9</f>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <f>C4*C9</f>
+        <v>18</v>
+      </c>
+      <c r="I14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14:J19" si="3">J3*$I$14</f>
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ref="K14:K19" si="4">J14/PI()</f>
+        <v>0.31830988618379069</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6">
-        <f>C3*C8</f>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>1600</v>
-      </c>
-      <c r="F7">
-        <f>F6/100</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <f>C7/C6</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C15">
+        <f>C14/1000</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>0.63661977236758138</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <f>1/C15</f>
+        <v>55.555555555555557</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>1.2732395447351628</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <f>C16*F5</f>
+        <v>888.88888888888891</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C10">
-        <f>C4*C8</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11">
-        <f>C10/1000</f>
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <f>1/(10^6)</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <f>C12/F3</f>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>2.5464790894703255</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <f>C17*F30</f>
+        <v>888.88888888888891</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14">
-        <f>C13*1000</f>
-        <v>16000</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15">
-        <f>C14/C10</f>
-        <v>400</v>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>5.0929581789406511</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>1.3</v>
+      </c>
+      <c r="H19">
+        <f>G19*F5</f>
+        <v>20.8</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>10.185916357881302</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>67</v>
+      </c>
+      <c r="D24">
+        <f>C24*(10^-6)</f>
+        <v>6.7000000000000002E-5</v>
+      </c>
+      <c r="E24">
+        <f>E25*F3</f>
+        <v>1.9999999999999998E-4</v>
+      </c>
+      <c r="F24">
+        <f>E24*(10^6)</f>
+        <v>199.99999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <f>D24/F3</f>
+        <v>1072</v>
+      </c>
+      <c r="E25">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31">
+        <f>F29*F30*F3</f>
+        <v>6.2500000000000001E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <f>F31*1000</f>
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of major changes to try things and experiment. Made everything global instead of in struct. Need to redo with fixed point math and continue code cleanup and changing things
</commit_message>
<xml_diff>
--- a/cycle_counts.xlsx
+++ b/cycle_counts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Projects\CNC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7EED8B-10FA-45E0-B346-E6423FA2FA1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BDB581-3593-4564-BA40-727DB86CED23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC3E716-96DC-4B36-BCEA-EA55029617FE}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="B2:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +478,7 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>5400</v>
+        <v>2200</v>
       </c>
       <c r="D2">
         <v>2100</v>
@@ -503,7 +503,7 @@
       </c>
       <c r="C3">
         <f>C2/60</f>
-        <v>90</v>
+        <v>36.666666666666664</v>
       </c>
       <c r="D3">
         <v>25</v>
@@ -537,7 +537,7 @@
       </c>
       <c r="C4">
         <f>C3/1000</f>
-        <v>0.09</v>
+        <v>3.6666666666666667E-2</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -568,7 +568,7 @@
       </c>
       <c r="C5">
         <f>C3/(10^6)</f>
-        <v>9.0000000000000006E-5</v>
+        <v>3.6666666666666666E-5</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -642,7 +642,7 @@
       </c>
       <c r="F8">
         <f>C13/100</f>
-        <v>180</v>
+        <v>73.333333333333329</v>
       </c>
       <c r="I8">
         <v>32</v>
@@ -670,7 +670,7 @@
       </c>
       <c r="F9">
         <f>C13/(10^6)</f>
-        <v>1.7999999999999999E-2</v>
+        <v>7.3333333333333332E-3</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -702,7 +702,7 @@
       </c>
       <c r="C12">
         <f>C13/C8</f>
-        <v>11.25</v>
+        <v>4.583333333333333</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -711,7 +711,7 @@
       </c>
       <c r="C13">
         <f>C3*C9</f>
-        <v>18000</v>
+        <v>7333.333333333333</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
@@ -720,7 +720,7 @@
       </c>
       <c r="C14">
         <f>C4*C9</f>
-        <v>18</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="I14">
         <v>5.0000000000000001E-3</v>
@@ -740,7 +740,7 @@
       </c>
       <c r="C15">
         <f>C14/1000</f>
-        <v>1.7999999999999999E-2</v>
+        <v>7.3333333333333332E-3</v>
       </c>
       <c r="J15">
         <f t="shared" si="3"/>
@@ -757,7 +757,7 @@
       </c>
       <c r="C16">
         <f>1/C15</f>
-        <v>55.555555555555557</v>
+        <v>136.36363636363637</v>
       </c>
       <c r="J16">
         <f t="shared" si="3"/>
@@ -774,7 +774,7 @@
       </c>
       <c r="C17">
         <f>C16*F5</f>
-        <v>888.88888888888891</v>
+        <v>2181.818181818182</v>
       </c>
       <c r="J17">
         <f t="shared" si="3"/>
@@ -791,7 +791,7 @@
       </c>
       <c r="C18">
         <f>C17*F30</f>
-        <v>888.88888888888891</v>
+        <v>2181.818181818182</v>
       </c>
       <c r="J18">
         <f t="shared" si="3"/>

</xml_diff>